<commit_message>
update documentation, update percentage calculation on figure
</commit_message>
<xml_diff>
--- a/global-summary/data/data dictionary.xlsx
+++ b/global-summary/data/data dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/NAPHS-data/global-summary/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4714289-CD02-C041-8427-A2D783FCD142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8734C900-61D2-3B4F-AEC0-DD1C5ABB84FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="199">
   <si>
     <t>Text</t>
   </si>
@@ -530,9 +530,6 @@
     <t>This data dictionary is intended to document the dataset(s) accessible at https://github.com/cghss/NAPHS-data</t>
   </si>
   <si>
-    <t>The data dictionary was last updated on September 8, 2023</t>
-  </si>
-  <si>
     <t>Country-level information, for each WHO Member State, on the status of JEE and NAPHS completion and reporting</t>
   </si>
   <si>
@@ -542,9 +539,6 @@
     <t>one-time (no updates)</t>
   </si>
   <si>
-    <t>See field information for more detail. Data extracted as of September 8, 2023 based on the most recently published data available on relevant WHO portals at that time.</t>
-  </si>
-  <si>
     <t>This is the primary key of this table. ISO 3166 codes are prepared by the International Organization for Standardization.</t>
   </si>
   <si>
@@ -627,6 +621,18 @@
   </si>
   <si>
     <t>Boolean (TRUE/FALSE) indicating whether the country published machine-readable (e.g., .csv, .tsv) line-item cost estimate as part of their published National Action Plan for Health Security (NAPHS) as of 8 September 2023, NULL if no NAPHS has been published</t>
+  </si>
+  <si>
+    <t>See field information for more detail. Data extracted as of September 8, 2023 based on the most recently published data available on relevant WHO portals at that time. Data were extracted by one member of the research team and then QA'ed/validated by a separate research team member.</t>
+  </si>
+  <si>
+    <t>The data dictionary was last updated on September 15, 2023</t>
+  </si>
+  <si>
+    <t>Added a note in "Table information" that data had been QA'ed/validated by a separate member of the research team</t>
+  </si>
+  <si>
+    <t>Clarification</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1158,7 @@
   <dimension ref="A2:W999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1162,7 +1168,7 @@
     <col min="3" max="3" width="47.59765625" customWidth="1"/>
     <col min="4" max="4" width="26.3984375" customWidth="1"/>
     <col min="5" max="5" width="28.59765625" customWidth="1"/>
-    <col min="6" max="6" width="58.19921875" customWidth="1"/>
+    <col min="6" max="6" width="80" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.25">
@@ -1176,7 +1182,7 @@
     </row>
     <row r="3" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -1229,24 +1235,24 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="16" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" s="16" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>146</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>165</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>166</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>148</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>168</v>
+        <v>195</v>
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
@@ -3333,8 +3339,8 @@
   </sheetPr>
   <dimension ref="A1:T815"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3392,7 +3398,7 @@
         <v>157</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
@@ -3421,10 +3427,10 @@
         <v>154</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
@@ -3485,10 +3491,10 @@
         <v>156</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
@@ -3514,13 +3520,13 @@
         <v>152</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" s="31" t="s">
         <v>171</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>173</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
@@ -3543,16 +3549,16 @@
         <v>146</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
@@ -3575,16 +3581,16 @@
         <v>146</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
@@ -3607,16 +3613,16 @@
         <v>146</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
@@ -3639,16 +3645,16 @@
         <v>146</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -3671,16 +3677,16 @@
         <v>146</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
@@ -4518,13 +4524,13 @@
   <dimension ref="A1:S998"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.19921875" customWidth="1"/>
-    <col min="2" max="2" width="36.59765625" customWidth="1"/>
+    <col min="2" max="2" width="52.59765625" customWidth="1"/>
     <col min="3" max="3" width="38.59765625" customWidth="1"/>
     <col min="4" max="4" width="48.796875" customWidth="1"/>
     <col min="5" max="5" width="57.59765625" customWidth="1"/>
@@ -4565,7 +4571,7 @@
         <v>44974</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>162</v>
@@ -4599,7 +4605,7 @@
         <v>160</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>161</v>
@@ -4623,11 +4629,21 @@
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="29">
+        <v>45177</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>145</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>

</xml_diff>